<commit_message>
agregado tutorial que se pasar en MKD y tambien las primeras migraciones y seeders
</commit_message>
<xml_diff>
--- a/db.xlsx
+++ b/db.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/46a54c639faf01ca/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taois\Documents\proyectos\python\uc_2024\hotel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="156" documentId="8_{931919D5-C5EA-4F05-BC21-FB7508B680C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{55652979-2664-4CDC-8C2D-C050A1D2D9B3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC06F1CF-AAF1-4DCB-B9F0-BC76AA0A266A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="3240" windowWidth="20325" windowHeight="15345" xr2:uid="{AC2DC5A2-68DD-47F9-84BB-A90CA22FACC1}"/>
+    <workbookView xWindow="14175" yWindow="2160" windowWidth="20325" windowHeight="15345" xr2:uid="{AC2DC5A2-68DD-47F9-84BB-A90CA22FACC1}"/>
   </bookViews>
   <sheets>
     <sheet name="hoteles" sheetId="1" r:id="rId1"/>
@@ -40,14 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>hoteles</t>
-  </si>
-  <si>
     <t>titulo</t>
   </si>
   <si>
@@ -109,6 +106,9 @@
   </si>
   <si>
     <t>id_serv_extra</t>
+  </si>
+  <si>
+    <t>nombre</t>
   </si>
 </sst>
 </file>
@@ -144,9 +144,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,58 +480,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23ADB6CC-BC6B-4215-9724-8A27B4F0922A}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B1" t="s">
+        <v>22</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="B2" t="s">
+        <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -559,13 +549,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -573,10 +563,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>50000</v>
@@ -587,10 +577,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>70000</v>
@@ -601,10 +591,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>120000</v>
@@ -630,10 +620,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -641,7 +631,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>10000</v>
@@ -652,7 +642,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>15000</v>
@@ -663,7 +653,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>20000</v>
@@ -692,13 +682,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -791,13 +781,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>